<commit_message>
Updated and added samples
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
+++ b/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
@@ -671,7 +671,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -684,9 +684,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -724,7 +724,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -796,7 +796,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -977,7 +977,7 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" style="6"/>
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="4">
-        <v>15.419249390939662</v>
+        <v>15.419249390939701</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1187,7 +1187,7 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="10" max="10" width="33.7109375" customWidth="1"/>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B15</f>
-        <v>15.36742804500903</v>
+        <v>15.367428045009069</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1389,7 +1389,7 @@
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
   </cols>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B26" s="1">
         <f>Input!B12*B25/1000</f>
-        <v>0.27754648903691392</v>
+        <v>0.27754648903691465</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>4.9014558472553658</v>
+        <v>4.9014558472553533</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Upgraded Excel UO to Spreadsheet UO, now supports ODS files and runs on Linux
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
+++ b/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="4">
-        <v>15.419249390939662</v>
+        <v>15.419249390939701</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B15</f>
-        <v>15.36742804500903</v>
+        <v>15.367428045009069</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B26" s="1">
         <f>Input!B12*B25/1000</f>
-        <v>0.27754648903691392</v>
+        <v>0.27754648903691465</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>4.9014558472553658</v>
+        <v>4.9014558472553533</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Upgrades to Spreadsheet UO
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
+++ b/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="4">
-        <v>15.419249390939701</v>
+        <v>1.8503099269127579</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="B6" s="1">
         <f>Input!B6+Calculations!B27</f>
-        <v>303.05145584725534</v>
+        <v>338.99546539379475</v>
       </c>
       <c r="C6" s="1">
         <f>Input!C6</f>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B15</f>
-        <v>15.367428045009069</v>
+        <v>1.7984885809821252</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B26" s="1">
         <f>Input!B12*B25/1000</f>
-        <v>0.27754648903691465</v>
+        <v>3.330557868442964E-2</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>4.9014558472553533</v>
+        <v>40.845465393794754</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Redesigned phase envelope utilities interface
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
+++ b/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="4">
-        <v>1.8503099269127579</v>
+        <v>15.419249390939662</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="B6" s="1">
         <f>Input!B6+Calculations!B27</f>
-        <v>338.99546539379475</v>
+        <v>303.05145584725534</v>
       </c>
       <c r="C6" s="1">
         <f>Input!C6</f>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B15</f>
-        <v>1.7984885809821252</v>
+        <v>15.36742804500903</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B26" s="1">
         <f>Input!B12*B25/1000</f>
-        <v>3.330557868442964E-2</v>
+        <v>0.27754648903691392</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>40.845465393794754</v>
+        <v>4.9014558472553658</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Fixed heat balance in PFR; Added more mouse double-click shortcuts to unit op editors; Minor bug fixes
</commit_message>
<xml_diff>
--- a/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
+++ b/DWSIM/bin/x86/Release/samples/Electrolysis.xlsx
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="B12" s="4">
-        <v>15.419249390939662</v>
+        <v>15.419249390939701</v>
       </c>
       <c r="H12" s="8"/>
     </row>
@@ -1354,7 +1354,7 @@
       </c>
       <c r="B12">
         <f>Input!B12+Calculations!B15</f>
-        <v>15.36742804500903</v>
+        <v>15.367428045009069</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B26" s="1">
         <f>Input!B12*B25/1000</f>
-        <v>0.27754648903691392</v>
+        <v>0.27754648903691465</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>53</v>
@@ -1608,7 +1608,7 @@
       </c>
       <c r="B27" s="1">
         <f>B23/B24/B26</f>
-        <v>4.9014558472553658</v>
+        <v>4.9014558472553533</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>55</v>

</xml_diff>